<commit_message>
add type and example columns to variable.xlsx
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/gulacsy_dominik_student_ceu_edu/Documents/1st_trimester/DA1/DA_team_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_F25DC773A252ABDACC1048E3215C7F9A5ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C933364-C969-4135-9709-6462ACC371A1}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC1048E3215C7F9A5ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12C8CB60-9ABE-4BBB-BD75-B0BADD3E351D}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="14370" windowHeight="10935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -118,13 +118,43 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>quantitative</t>
+  </si>
+  <si>
+    <t>qualitative, nominal</t>
+  </si>
+  <si>
+    <t>qualitative, ordered</t>
+  </si>
+  <si>
+    <t>quantitative, ordered</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Cafe de Paris Pizza &amp; More</t>
+  </si>
+  <si>
+    <t>Budapest, Vörösmarty tér 1, 1051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.netpincer.hu/restaurant/v4sc/cafe-de-paris-pizza-and-more#restaurant-info </t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +169,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -199,10 +237,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -216,17 +255,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,148 +540,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>47.496670000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <v>19.050049999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="D16" s="4">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" location="restaurant-info " xr:uid="{0807F004-E2EF-4A1A-A8D2-6EF33675C41E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add data_type to variable.xlsx
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/gulacsy_dominik_student_ceu_edu/Documents/1st_trimester/DA1/DA_team_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrae\OneDrive\Bureau\CEU\DA1\DA_team_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC1048E3215C7F9A5ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12C8CB60-9ABE-4BBB-BD75-B0BADD3E351D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1C9FAD-2CD9-4C44-88E4-5DD8D09A05F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="14370" windowHeight="10935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="var_explanation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>example</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>data_type</t>
   </si>
 </sst>
 </file>
@@ -540,21 +549,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="5" max="5" width="83.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -562,13 +571,16 @@
         <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -576,69 +588,84 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -646,13 +673,16 @@
         <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>47.496670000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -660,13 +690,16 @@
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>19.050049999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -674,13 +707,16 @@
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -688,13 +724,16 @@
         <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -702,13 +741,16 @@
         <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -716,13 +758,16 @@
         <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>0.875</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -730,13 +775,16 @@
         <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -744,13 +792,16 @@
         <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>890</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -758,13 +809,16 @@
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -772,25 +826,28 @@
         <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J18" s="5"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K18" s="5"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="5"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" location="restaurant-info " xr:uid="{0807F004-E2EF-4A1A-A8D2-6EF33675C41E}"/>
+    <hyperlink ref="E5" r:id="rId1" location="restaurant-info " xr:uid="{0807F004-E2EF-4A1A-A8D2-6EF33675C41E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
Add variable type_beverage and category_beverage
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\OneDrive - Central European University\1st_trimester\DA1\DA_team_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrae\OneDrive\Bureau\CEU\DA1\DA_team_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A420D70-4833-4A5D-98A2-13A476496BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796F7E69-8AAB-475C-8A9D-28FEC4507BD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12075" yWindow="3270" windowWidth="14370" windowHeight="10935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="var_explanation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>type_beverage</t>
+  </si>
+  <si>
+    <t>Type of beverage</t>
+  </si>
+  <si>
+    <t>Pespi</t>
+  </si>
+  <si>
+    <t>Category of beverage</t>
+  </si>
+  <si>
+    <t>Soft</t>
+  </si>
+  <si>
+    <t>category_beverage</t>
   </si>
 </sst>
 </file>
@@ -200,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -248,12 +266,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -269,6 +296,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -552,21 +582,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="3" width="23.109375" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
-    <col min="5" max="5" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -583,7 +613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -600,7 +630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -617,7 +647,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -634,7 +664,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -651,7 +681,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -668,7 +698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -685,7 +715,7 @@
         <v>47.496670000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -702,7 +732,7 @@
         <v>19.050049999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -719,7 +749,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -736,7 +766,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -753,7 +783,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -770,7 +800,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -787,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -804,7 +834,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -821,32 +851,66 @@
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E18" s="4">
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add new variable: type_bev and category_bev
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrae\OneDrive\Bureau\CEU\DA1\DA_team_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796F7E69-8AAB-475C-8A9D-28FEC4507BD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04437BF5-7D6E-4C3F-ADF3-617DCB0BE4B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,9 +162,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>type_beverage</t>
-  </si>
-  <si>
     <t>Type of beverage</t>
   </si>
   <si>
@@ -177,7 +174,10 @@
     <t>Soft</t>
   </si>
   <si>
-    <t>category_beverage</t>
+    <t>type_bev</t>
+  </si>
+  <si>
+    <t>category_bev</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +853,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
@@ -862,10 +862,10 @@
         <v>43</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -879,10 +879,10 @@
         <v>43</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>